<commit_message>
changes in requirement file
</commit_message>
<xml_diff>
--- a/requirement/requirement.xlsx
+++ b/requirement/requirement.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dhruv\School management\school-management\requirement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4480E0AA-8138-4485-8CD6-0595538ACD9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D73C689C-F3B1-4567-B08C-B86FD39EB745}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirement" sheetId="1" r:id="rId1"/>
     <sheet name="Admin Modules" sheetId="2" r:id="rId2"/>
+    <sheet name="Branches" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="142">
   <si>
     <t>Requiremenmts</t>
   </si>
@@ -604,6 +605,177 @@
   </si>
   <si>
     <t>userId(to map student to whom room alloted)</t>
+  </si>
+  <si>
+    <t>1. Admin</t>
+  </si>
+  <si>
+    <t>1.1 Parents</t>
+  </si>
+  <si>
+    <t>1.2 Teachers</t>
+  </si>
+  <si>
+    <t>1.3 Students</t>
+  </si>
+  <si>
+    <t>1.4 Working Staff</t>
+  </si>
+  <si>
+    <t>1.1.1 Childrens</t>
+  </si>
+  <si>
+    <t>1.3.1 Time Table</t>
+  </si>
+  <si>
+    <t>1.3.2 Events</t>
+  </si>
+  <si>
+    <t>1.2.1 Classes assigned</t>
+  </si>
+  <si>
+    <t>1.2.2 Subjects assigned</t>
+  </si>
+  <si>
+    <t>1.2.3 Time table</t>
+  </si>
+  <si>
+    <t>1.2.4 Events</t>
+  </si>
+  <si>
+    <t>1.2.5 Notification(if any send by principal)</t>
+  </si>
+  <si>
+    <t>1.1.2 Teacher assigned to students class</t>
+  </si>
+  <si>
+    <t>1.1.3 Time table</t>
+  </si>
+  <si>
+    <t>1.1.4 Subjects assigned</t>
+  </si>
+  <si>
+    <t>1.1.5 Events</t>
+  </si>
+  <si>
+    <t>1.1.6 Notification</t>
+  </si>
+  <si>
+    <t>1.1.7 fees</t>
+  </si>
+  <si>
+    <t>1.3.3 Notification</t>
+  </si>
+  <si>
+    <t>1.3.4 Subjects</t>
+  </si>
+  <si>
+    <t>1.3.5 Fees</t>
+  </si>
+  <si>
+    <t>1.5 Departments</t>
+  </si>
+  <si>
+    <t>1.6 Hostel</t>
+  </si>
+  <si>
+    <t>1.7 Transportation</t>
+  </si>
+  <si>
+    <t>1.8 Accounts</t>
+  </si>
+  <si>
+    <t>1.9 Subjects</t>
+  </si>
+  <si>
+    <t>1.10 Class</t>
+  </si>
+  <si>
+    <t>1.11 Holidays</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.12 Fees </t>
+  </si>
+  <si>
+    <t>1.13 Library</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.14 Exam </t>
+  </si>
+  <si>
+    <t>1.15 Time Table</t>
+  </si>
+  <si>
+    <t>1.16 Events</t>
+  </si>
+  <si>
+    <t>1.17 Printing</t>
+  </si>
+  <si>
+    <t>1.18 Blog</t>
+  </si>
+  <si>
+    <t>1.2.6 Attendance</t>
+  </si>
+  <si>
+    <t>1.3.6 Attendance</t>
+  </si>
+  <si>
+    <t>1.1.8 Attendance</t>
+  </si>
+  <si>
+    <t>1.19 Notice</t>
+  </si>
+  <si>
+    <t>1.20 Message</t>
+  </si>
+  <si>
+    <t>1.1.9 Profile(self, childrens)</t>
+  </si>
+  <si>
+    <t>1.3.7 Self Profile</t>
+  </si>
+  <si>
+    <t>1.3.8 Exams, Exam result</t>
+  </si>
+  <si>
+    <t>1.1.10 Exam, Exam result</t>
+  </si>
+  <si>
+    <t>1.2.7 Salary</t>
+  </si>
+  <si>
+    <t>1.2.8 Exams</t>
+  </si>
+  <si>
+    <t>1.4.1 Salary</t>
+  </si>
+  <si>
+    <t>1.4.2 Notification</t>
+  </si>
+  <si>
+    <t>1.6.1 Room alloting</t>
+  </si>
+  <si>
+    <t>1.6.2 Total student</t>
+  </si>
+  <si>
+    <t>1.6.3 Fees Paid or unpaid</t>
+  </si>
+  <si>
+    <t>1.6.4 Query module</t>
+  </si>
+  <si>
+    <t>1.3.9 Query raise against hostel</t>
+  </si>
+  <si>
+    <t>1.8.1 Slary of staff</t>
+  </si>
+  <si>
+    <t>1.8.2 Fees of student</t>
+  </si>
+  <si>
+    <t>1.8.3 Expenses</t>
   </si>
 </sst>
 </file>
@@ -941,7 +1113,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
@@ -1423,4 +1595,235 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CA302E6-A7D2-4147-907D-75705999803A}">
+  <dimension ref="A1:U11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L1" sqref="A1:U11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G1" t="s">
+        <v>108</v>
+      </c>
+      <c r="H1" t="s">
+        <v>109</v>
+      </c>
+      <c r="I1" t="s">
+        <v>110</v>
+      </c>
+      <c r="J1" t="s">
+        <v>111</v>
+      </c>
+      <c r="K1" t="s">
+        <v>112</v>
+      </c>
+      <c r="L1" t="s">
+        <v>113</v>
+      </c>
+      <c r="M1" t="s">
+        <v>114</v>
+      </c>
+      <c r="N1" t="s">
+        <v>115</v>
+      </c>
+      <c r="O1" t="s">
+        <v>116</v>
+      </c>
+      <c r="P1" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>118</v>
+      </c>
+      <c r="R1" t="s">
+        <v>119</v>
+      </c>
+      <c r="S1" t="s">
+        <v>120</v>
+      </c>
+      <c r="T1" t="s">
+        <v>124</v>
+      </c>
+      <c r="U1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E2" t="s">
+        <v>132</v>
+      </c>
+      <c r="G2" t="s">
+        <v>134</v>
+      </c>
+      <c r="I2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D3" t="s">
+        <v>92</v>
+      </c>
+      <c r="E3" t="s">
+        <v>133</v>
+      </c>
+      <c r="G3" t="s">
+        <v>135</v>
+      </c>
+      <c r="I3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C4" t="s">
+        <v>95</v>
+      </c>
+      <c r="D4" t="s">
+        <v>104</v>
+      </c>
+      <c r="G4" t="s">
+        <v>136</v>
+      </c>
+      <c r="I4" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D5" t="s">
+        <v>105</v>
+      </c>
+      <c r="G5" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>101</v>
+      </c>
+      <c r="C6" t="s">
+        <v>97</v>
+      </c>
+      <c r="D6" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>102</v>
+      </c>
+      <c r="C7" t="s">
+        <v>121</v>
+      </c>
+      <c r="D7" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>103</v>
+      </c>
+      <c r="C8" t="s">
+        <v>130</v>
+      </c>
+      <c r="D8" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>123</v>
+      </c>
+      <c r="C9" t="s">
+        <v>131</v>
+      </c>
+      <c r="D9" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>126</v>
+      </c>
+      <c r="D10" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>129</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>